<commit_message>
modification on util functionality
</commit_message>
<xml_diff>
--- a/src/testdata.xlsx
+++ b/src/testdata.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>collection_Name</t>
   </si>
@@ -30,9 +30,6 @@
     <t>testIterationCount</t>
   </si>
   <si>
-    <t>folder_name</t>
-  </si>
-  <si>
     <t>Environment-UAT</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
     <t>ServiceName_JenkinsParam</t>
   </si>
   <si>
-    <t>NextGen-userRequests</t>
-  </si>
-  <si>
     <t>NormalUserRequests</t>
   </si>
   <si>
@@ -70,6 +64,18 @@
   </si>
   <si>
     <t>createuser/Demodata.json</t>
+  </si>
+  <si>
+    <t>DemoCollection2.postman_collection.json</t>
+  </si>
+  <si>
+    <t>RecieveDataRequests</t>
+  </si>
+  <si>
+    <t>ReceiveDataRequests.html</t>
+  </si>
+  <si>
+    <t>receivedata</t>
   </si>
 </sst>
 </file>
@@ -387,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,16 +404,15 @@
     <col min="1" max="1" width="45.140625" customWidth="1"/>
     <col min="2" max="2" width="37.85546875" customWidth="1"/>
     <col min="3" max="3" width="26.28515625" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" customWidth="1"/>
-    <col min="6" max="6" width="42.85546875" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
-    <col min="9" max="9" width="35.7109375" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="42.85546875" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+    <col min="8" max="8" width="35.7109375" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,31 +440,45 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
       </c>
       <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>